<commit_message>
Update database Update Tracking Process.xlsx
</commit_message>
<xml_diff>
--- a/Tracking Process.xlsx
+++ b/Tracking Process.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Info" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Server LMS" sheetId="4" r:id="rId5"/>
     <sheet name="GateWay" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -256,12 +256,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -279,6 +273,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,23 +636,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="48" customHeight="1">
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="D3" s="4"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="D5" s="5"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="D6" s="5"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -724,111 +724,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -855,159 +855,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="60">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>40277</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7" t="s">
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>